<commit_message>
LH local- new figs
Standardized colors, did some palette work
Got pdfs in a nice place figure-wise
Still thinking about family level- to keep without se bars, maybe remove legend?
</commit_message>
<xml_diff>
--- a/Mosquito Life history colab/Life history local/GEI/Nydar local GEI composite.xlsx
+++ b/Mosquito Life history colab/Life history local/GEI/Nydar local GEI composite.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgc\Documents\GitHub\wingproj\Mosquito Life history colab\Life history local\GEI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Documents\GitHub\wingproj\Mosquito Life history colab\Life history local\GEI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130AD61E-38BE-4BE8-80B6-895EABE89589}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{79C102A5-8550-4547-BD91-AAD0DD29EBF4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13410" windowHeight="9300" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2613,8 +2613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D90C63-E797-48CF-9837-6227D64C602D}">
   <dimension ref="B2:AF47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2634,7 +2634,7 @@
     <col min="24" max="25" width="9.140625" style="10"/>
     <col min="26" max="26" width="20.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="27" max="30" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="32" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>

</xml_diff>